<commit_message>
Final Revisions, plan to consolidate notebooks
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR1986-01-31-2006-01-31.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR1986-01-31-2006-01-31.xlsx
@@ -14,24 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>C_B</t>
+  </si>
+  <si>
+    <t>C_LF</t>
+  </si>
   <si>
     <t>FFR_B</t>
   </si>
   <si>
-    <t>FFR_C</t>
-  </si>
-  <si>
     <t>FFR_LF</t>
-  </si>
-  <si>
-    <t>C_B</t>
-  </si>
-  <si>
-    <t>C_FFR</t>
-  </si>
-  <si>
-    <t>C_LF</t>
   </si>
   <si>
     <t>params</t>
@@ -395,13 +389,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,57 +408,39 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2">
+        <v>0.87504171261757</v>
+      </c>
+      <c r="C2">
+        <v>0.00337956661413657</v>
+      </c>
+      <c r="D2">
+        <v>-18.0515008959796</v>
+      </c>
+      <c r="E2">
+        <v>0.4919540470472872</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>-31.39121201093776</v>
-      </c>
-      <c r="C2">
-        <v>14.63657399565489</v>
-      </c>
-      <c r="D2">
-        <v>0.8120107323222316</v>
-      </c>
-      <c r="E2">
-        <v>0.9304207327887289</v>
-      </c>
-      <c r="F2">
-        <v>0.003332168454532673</v>
-      </c>
-      <c r="G2">
-        <v>0.001955766707789976</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B3">
-        <v>8.43769498715119E-14</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.0005175079872536958</v>
+        <v>5.788347579027686E-11</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0.0005175079872530297</v>
-      </c>
-      <c r="G3">
-        <v>0.1387040414342497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>